<commit_message>
rpr server publishes real msg
</commit_message>
<xml_diff>
--- a/blueprint_raw.xlsx
+++ b/blueprint_raw.xlsx
@@ -126,69 +126,39 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
-      <c r="B1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>0</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
succesfully restored working state of tb3
</commit_message>
<xml_diff>
--- a/blueprint_raw.xlsx
+++ b/blueprint_raw.xlsx
@@ -17,6 +17,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t xml:space="preserve">stack list</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -126,14 +134,14 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="n">
-        <v>4</v>
+      <c r="A1" s="0" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -141,28 +149,36 @@
       <c r="E1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="n">
+        <v>3</v>
+      </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>

</xml_diff>